<commit_message>
Update DR# 743 Wildflour (Loyalty Card) 7-19-22.xlsx
</commit_message>
<xml_diff>
--- a/DR# 743 Wildflour (Loyalty Card) 7-19-22.xlsx
+++ b/DR# 743 Wildflour (Loyalty Card) 7-19-22.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JIM\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UBIVELOX\Documents\GitHub\Delivery-Receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF89FEA-C31D-4794-9500-CF673A4573EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$26</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>DELIVERY RECEIPT</t>
   </si>
@@ -46,15 +45,6 @@
   </si>
   <si>
     <t>DATE RECEIVED</t>
-  </si>
-  <si>
-    <t>Unit 7D Strata 100 Building, Emerald Avenue,</t>
-  </si>
-  <si>
-    <t>Ortigas Center, Pasig City</t>
-  </si>
-  <si>
-    <t>Tel. No. (02) 954-2719</t>
   </si>
   <si>
     <t>Total:</t>
@@ -97,12 +87,6 @@
     <t>Cards</t>
   </si>
   <si>
-    <t>Address: Six / Neo 4th Avenue corner 26th St. Bonifacio Global City, Taguig</t>
-  </si>
-  <si>
-    <t>TO:  Wildflour</t>
-  </si>
-  <si>
     <t>Loyalty Card</t>
   </si>
   <si>
@@ -128,11 +112,46 @@
       <t xml:space="preserve"> 000743</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Address: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Six / Neo 4th Avenue corner 26th St. Bonifacio Global City, Taguig</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wildflour Bakery &amp; Café Corp</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit 7D Strata 100 Building, Emerald Avenue, Ortigas Center, Pasig City
+Tel. No. (02) 954-2719
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -343,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -391,13 +410,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -509,7 +538,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -544,7 +573,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -728,11 +757,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:M25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -744,29 +773,32 @@
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:13">
+      <c r="D1" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="27"/>
+    </row>
     <row r="2" spans="1:13">
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="7" spans="1:13" ht="50.25" customHeight="1">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -787,41 +819,35 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="21" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="2"/>
-    </row>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="21" customHeight="1"/>
     <row r="11" spans="1:13" ht="21" customHeight="1">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:13" ht="18.75">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
     </row>
     <row r="13" spans="1:13" ht="19.5" thickBot="1">
       <c r="A13" s="2"/>
@@ -849,10 +875,10 @@
     </row>
     <row r="15" spans="1:13" ht="18.75">
       <c r="A15" s="22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C15" s="15">
         <v>10000</v>
@@ -901,10 +927,13 @@
     </row>
     <row r="21" spans="1:5" ht="18.75">
       <c r="A21" s="11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
+      <c r="C21" s="28">
+        <f>C15</f>
+        <v>10000</v>
+      </c>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
     </row>
@@ -916,14 +945,17 @@
       <c r="E22" s="14"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
+      <c r="C25" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A11:M11"/>
+    <mergeCell ref="D1:E4"/>
+    <mergeCell ref="C25:E25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>